<commit_message>
updated cnic missing list
</commit_message>
<xml_diff>
--- a/data/missing_cnics_categorized.xlsx
+++ b/data/missing_cnics_categorized.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="missing_cnics" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">missing_cnics!$A$1:$H$130</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="234">
   <si>
     <t>seat_id</t>
   </si>
@@ -392,6 +395,330 @@
   </si>
   <si>
     <t>could also be 3310022229145</t>
+  </si>
+  <si>
+    <t>PP-32</t>
+  </si>
+  <si>
+    <t>Sharafat hussain</t>
+  </si>
+  <si>
+    <t>PP-147</t>
+  </si>
+  <si>
+    <t>Asghar butt</t>
+  </si>
+  <si>
+    <t>PP-204</t>
+  </si>
+  <si>
+    <t>Abbas zafar haraj</t>
+  </si>
+  <si>
+    <t>PP-148</t>
+  </si>
+  <si>
+    <t>Aloudin</t>
+  </si>
+  <si>
+    <t>NA-106</t>
+  </si>
+  <si>
+    <t>Nisar Ahmad</t>
+  </si>
+  <si>
+    <t>PP-101</t>
+  </si>
+  <si>
+    <t>Rai Ijaz Hussain</t>
+  </si>
+  <si>
+    <t>Rai Haider Ali Khan</t>
+  </si>
+  <si>
+    <t>PP-224</t>
+  </si>
+  <si>
+    <t>Mian Amir Iqbal Shah</t>
+  </si>
+  <si>
+    <t>Saira</t>
+  </si>
+  <si>
+    <t>NA-83</t>
+  </si>
+  <si>
+    <t>PP-122</t>
+  </si>
+  <si>
+    <t>Nazia raheel</t>
+  </si>
+  <si>
+    <t>Shahid Mehmood</t>
+  </si>
+  <si>
+    <t>PP-149</t>
+  </si>
+  <si>
+    <t>Abdul Hameed</t>
+  </si>
+  <si>
+    <t>PP-276</t>
+  </si>
+  <si>
+    <t>Mian  Khizar</t>
+  </si>
+  <si>
+    <t>Amjid  Ali</t>
+  </si>
+  <si>
+    <t>PP-278</t>
+  </si>
+  <si>
+    <t>Najeeb  ur  Rheman</t>
+  </si>
+  <si>
+    <t>Muhammad  Ayub</t>
+  </si>
+  <si>
+    <t>Mian Amir  Sultan</t>
+  </si>
+  <si>
+    <t>NA-144</t>
+  </si>
+  <si>
+    <t>Muhhamad jamil ashraf</t>
+  </si>
+  <si>
+    <t>Shehzad zulfiqar</t>
+  </si>
+  <si>
+    <t>PP-183</t>
+  </si>
+  <si>
+    <t>Syed saqlain</t>
+  </si>
+  <si>
+    <t>Nisar tanveer</t>
+  </si>
+  <si>
+    <t>Rahila anwar</t>
+  </si>
+  <si>
+    <t>Dr.yasmeen rana</t>
+  </si>
+  <si>
+    <t>NA-156</t>
+  </si>
+  <si>
+    <t>Makhdoom Shah Mahmood Hudsaini Qureshi</t>
+  </si>
+  <si>
+    <t>NA-64</t>
+  </si>
+  <si>
+    <t>abdul satar</t>
+  </si>
+  <si>
+    <t>tahir iqbal</t>
+  </si>
+  <si>
+    <t>PP-201</t>
+  </si>
+  <si>
+    <t>Muhammad Iqbal</t>
+  </si>
+  <si>
+    <t>NA-77</t>
+  </si>
+  <si>
+    <t>Muhammad Ashfaq Taj</t>
+  </si>
+  <si>
+    <t>PP-26</t>
+  </si>
+  <si>
+    <t>M. Arif</t>
+  </si>
+  <si>
+    <t>PP-27</t>
+  </si>
+  <si>
+    <t>Raheela anwar</t>
+  </si>
+  <si>
+    <t>NA-146</t>
+  </si>
+  <si>
+    <t>Rana zahid hussain khan</t>
+  </si>
+  <si>
+    <t>PP-160</t>
+  </si>
+  <si>
+    <t>Akhartar mehmood</t>
+  </si>
+  <si>
+    <t>PP-92</t>
+  </si>
+  <si>
+    <t>Malik mehboob Ahmad</t>
+  </si>
+  <si>
+    <t>Nasreen riaz</t>
+  </si>
+  <si>
+    <t>Sadia nadeem malik</t>
+  </si>
+  <si>
+    <t>PP-117</t>
+  </si>
+  <si>
+    <t>M islam</t>
+  </si>
+  <si>
+    <t>Mian Muhammad Bahadur</t>
+  </si>
+  <si>
+    <t>Saira Bano</t>
+  </si>
+  <si>
+    <t>PP-150</t>
+  </si>
+  <si>
+    <t>Bilal Yasin</t>
+  </si>
+  <si>
+    <t>PP-57</t>
+  </si>
+  <si>
+    <t>Ashraf ali</t>
+  </si>
+  <si>
+    <t>PK-31</t>
+  </si>
+  <si>
+    <t>Sardar zahoor ahmed</t>
+  </si>
+  <si>
+    <t>PP-30</t>
+  </si>
+  <si>
+    <t>zafar ullah khan</t>
+  </si>
+  <si>
+    <t>Zakia khan</t>
+  </si>
+  <si>
+    <t>PP-102</t>
+  </si>
+  <si>
+    <t>Ehsan Mushtaq Toor</t>
+  </si>
+  <si>
+    <t>NA-147</t>
+  </si>
+  <si>
+    <t>Syed Imran Ahmad Shah</t>
+  </si>
+  <si>
+    <t>NA-149</t>
+  </si>
+  <si>
+    <t>Shahnaz Javed</t>
+  </si>
+  <si>
+    <t>NA-109</t>
+  </si>
+  <si>
+    <t>Mohsin Raza</t>
+  </si>
+  <si>
+    <t>Shiekh Ijaz Ahmad</t>
+  </si>
+  <si>
+    <t>NA-110</t>
+  </si>
+  <si>
+    <t>Muhammad ilyas</t>
+  </si>
+  <si>
+    <t>PP-184</t>
+  </si>
+  <si>
+    <t>Syed ali rayaz</t>
+  </si>
+  <si>
+    <t>PP-185</t>
+  </si>
+  <si>
+    <t>Sardar muhamad saeed</t>
+  </si>
+  <si>
+    <t>NA-86</t>
+  </si>
+  <si>
+    <t>Fakkhar Umar Hayyat</t>
+  </si>
+  <si>
+    <t>PP-65</t>
+  </si>
+  <si>
+    <t>Tariq Mahmood</t>
+  </si>
+  <si>
+    <t>PP-66</t>
+  </si>
+  <si>
+    <t>Syed Tariq Yaqoob</t>
+  </si>
+  <si>
+    <t>NA-157</t>
+  </si>
+  <si>
+    <t>Sayed ali moosa gilani</t>
+  </si>
+  <si>
+    <t>NA-158</t>
+  </si>
+  <si>
+    <t>Muhammad Ibrahim Khan</t>
+  </si>
+  <si>
+    <t>Makhdoom Muhammad Javed Hashmi</t>
+  </si>
+  <si>
+    <t>NA-159</t>
+  </si>
+  <si>
+    <t>Dewan Ashiq Hussain Bukhari</t>
+  </si>
+  <si>
+    <t>PK-71</t>
+  </si>
+  <si>
+    <t>Javed khan momen</t>
+  </si>
+  <si>
+    <t>Shah farmaan</t>
+  </si>
+  <si>
+    <t>PK-72</t>
+  </si>
+  <si>
+    <t>Kashif azam</t>
+  </si>
+  <si>
+    <t>PK-4</t>
+  </si>
+  <si>
+    <t>Amir muqam</t>
+  </si>
+  <si>
+    <t>PP-22</t>
+  </si>
+  <si>
+    <t>tanveer aslam</t>
   </si>
 </sst>
 </file>
@@ -1227,21 +1554,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="55.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1255,7 +1582,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1273,62 +1600,62 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3130196190263</v>
+        <v>30</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3320110081825</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3120196190263</v>
+        <v>60</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3320110081825</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2">
-        <v>935</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3120244368991</v>
+        <v>57</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3310406902731</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3120244368991</v>
+        <v>59</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3310406902331</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C4" s="2">
-        <v>8253</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3220364078687</v>
+        <v>88</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3310007903593</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1337,116 +1664,89 @@
         <v>59</v>
       </c>
       <c r="G4" s="1">
-        <v>3220364078087</v>
+        <v>3310070790359</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8468</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3240486787951</v>
+        <v>135</v>
+      </c>
+      <c r="C5">
+        <v>96</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3310080556595</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="1">
-        <v>3240480787951</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3320110081825</v>
+        <v>204</v>
+      </c>
+      <c r="C6">
+        <v>-9999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3310096538007</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="3">
-        <v>3320110081825</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2">
-        <v>9441</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3310147826873</v>
+        <v>205</v>
+      </c>
+      <c r="C7">
+        <v>-9999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3310045508655</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3310147896873</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3460357085705</v>
+        <v>207</v>
+      </c>
+      <c r="C8">
+        <v>-9999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3310063074697</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3460357086705</v>
-      </c>
-      <c r="H8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2">
-        <v>8099</v>
-      </c>
-      <c r="D9" s="3">
-        <v>3330416456315</v>
+        <v>-9999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3540169000129</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1455,44 +1755,44 @@
         <v>59</v>
       </c>
       <c r="G9" s="1">
-        <v>3230416456315</v>
+        <v>3540169800129</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2">
-        <v>8082</v>
-      </c>
-      <c r="D10" s="3">
-        <v>3230460778535</v>
+        <v>267</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3540115035463</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="3">
-        <v>3230460778535</v>
+        <v>59</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3540115035465</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2">
-        <v>8096</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3230425492523</v>
+        <v>559</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3520115279207</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -1501,21 +1801,21 @@
         <v>59</v>
       </c>
       <c r="G11" s="1">
-        <v>3230425492253</v>
+        <v>3520116279207</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3230968844001</v>
+        <v>5567</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -1524,139 +1824,106 @@
         <v>59</v>
       </c>
       <c r="G12" s="1">
-        <v>3230468844001</v>
+        <v>9999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2">
-        <v>8001</v>
-      </c>
-      <c r="D13" s="3">
-        <v>3234564196655</v>
+        <v>156</v>
+      </c>
+      <c r="C13">
+        <v>591</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3530151347383</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="1">
-        <v>3230456419665</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2330492812615</v>
+        <v>157</v>
+      </c>
+      <c r="C14">
+        <v>596</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3530144305577</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3230482812615</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="2">
-        <v>57</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3310406902731</v>
+        <v>177</v>
+      </c>
+      <c r="C15">
+        <v>-9999</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3520266391347</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3310406902331</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D16" s="3">
-        <v>3720212416532</v>
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>636</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3650226673435</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3120212416532</v>
-      </c>
-      <c r="H16" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3310074119078</v>
+        <v>202</v>
+      </c>
+      <c r="C17">
+        <v>-9999</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3620281727692</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3310074119878</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2">
-        <v>848</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3520104396883</v>
+        <v>680</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3630278115075</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
@@ -1664,11 +1931,8 @@
       <c r="F18" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="1">
-        <v>3520104396583</v>
-      </c>
-      <c r="H18" t="s">
-        <v>122</v>
+      <c r="G18" s="3">
+        <v>3630278115075</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1681,7 +1945,7 @@
       <c r="C19" s="2">
         <v>701</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="1">
         <v>3630248950581</v>
       </c>
       <c r="E19" t="b">
@@ -1704,7 +1968,7 @@
       <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="1">
         <v>3630264299811</v>
       </c>
       <c r="E20" t="b">
@@ -1727,7 +1991,7 @@
       <c r="C21" s="2">
         <v>713</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="1">
         <v>3630249481473</v>
       </c>
       <c r="E21" t="b">
@@ -1742,240 +2006,219 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2">
-        <v>680</v>
-      </c>
-      <c r="D22" s="3">
-        <v>3630278115075</v>
+        <v>97</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3630297069351</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="3">
-        <v>3630278115075</v>
+        <v>59</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3630297009391</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="2">
-        <v>558</v>
-      </c>
-      <c r="D23" s="3">
-        <v>3530020775569</v>
+        <v>98</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3630224801051</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="1">
+        <v>3630224801851</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="2">
-        <v>559</v>
-      </c>
-      <c r="D24" s="3">
-        <v>3520115279207</v>
+        <v>164</v>
+      </c>
+      <c r="C24">
+        <v>733</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3630203044371</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="1">
-        <v>3520116279207</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>218</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="2">
-        <v>5567</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
+        <v>219</v>
+      </c>
+      <c r="C25">
+        <v>740</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3520126954701</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="1">
-        <v>9999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="2">
-        <v>175</v>
-      </c>
-      <c r="D26" s="3">
-        <v>3330332918642</v>
+        <v>221</v>
+      </c>
+      <c r="C26">
+        <v>752</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3630291706293</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="1">
-        <v>3330382918642</v>
-      </c>
-      <c r="H26" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="2">
-        <v>267</v>
-      </c>
-      <c r="D27" s="3">
-        <v>3540115035463</v>
+        <v>222</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3630320525349</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" s="1">
-        <v>3540115035465</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D28" s="3">
-        <v>3740287478099</v>
+        <v>224</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3630198902051</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" s="1">
-        <v>3740587478099</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2">
-        <v>2920</v>
-      </c>
-      <c r="D29" s="3">
-        <v>6110136279375</v>
+        <v>848</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3520104396883</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G29" s="1">
-        <v>6110136277375</v>
+        <v>3520104396583</v>
+      </c>
+      <c r="H29" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C30" s="2">
         <v>-9999</v>
       </c>
-      <c r="D30" s="3">
-        <v>6110119162492</v>
+      <c r="D30" s="1">
+        <v>3130196190263</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3120196190263</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C31" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3520228850587</v>
+        <v>935</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3120244368991</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G31" s="3">
-        <v>3520228850581</v>
-      </c>
-      <c r="H31" t="s">
-        <v>124</v>
+        <v>3120244368991</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C32" s="2">
         <v>-9999</v>
       </c>
-      <c r="D32" s="3">
-        <v>3520241959731</v>
+      <c r="D32" s="1">
+        <v>3740287478099</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -1984,21 +2227,21 @@
         <v>59</v>
       </c>
       <c r="G32" s="1">
-        <v>3420241959731</v>
+        <v>3740587478099</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C33" s="2">
-        <v>8547</v>
-      </c>
-      <c r="D33" s="3">
-        <v>3420206866313</v>
+        <v>2920</v>
+      </c>
+      <c r="D33" s="1">
+        <v>6110136279375</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -2007,113 +2250,95 @@
         <v>59</v>
       </c>
       <c r="G33" s="1">
-        <v>3420206866713</v>
+        <v>6110136277375</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D34" s="3">
-        <v>9110901034965</v>
+        <v>166</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3070215167855</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="1">
-        <v>9110901034695</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D35" s="3">
-        <v>3120203176499</v>
+        <v>167</v>
+      </c>
+      <c r="C35">
+        <v>-9999</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3722010788414</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>60</v>
-      </c>
-      <c r="G35" s="3">
-        <v>3120203176499</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D36" s="3">
-        <v>3120202690303</v>
+        <v>3032</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3730333449105</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>60</v>
-      </c>
-      <c r="G36" s="3">
-        <v>3120202690303</v>
+        <v>59</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3730333448105</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="2">
-        <v>7801</v>
-      </c>
-      <c r="D37" s="3">
-        <v>3120558226560</v>
+        <v>171</v>
+      </c>
+      <c r="C37">
+        <v>3155</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3450261850143</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
-      </c>
-      <c r="F37" t="s">
-        <v>59</v>
-      </c>
-      <c r="G37" s="1">
-        <v>3120258226560</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D38" s="3">
-        <v>3460107505057</v>
+        <v>64</v>
+      </c>
+      <c r="C38">
+        <v>3258</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3410270899731</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
@@ -2121,180 +2346,135 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>212</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D39" s="3">
-        <v>3520233441959</v>
+        <v>213</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3520096685423</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>59</v>
-      </c>
-      <c r="G39" s="1">
-        <v>3520252451959</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="2">
-        <v>8771</v>
-      </c>
-      <c r="D40" s="3">
-        <v>3410422858955</v>
+        <v>193</v>
+      </c>
+      <c r="C40">
+        <v>4620</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4230180790699</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-      <c r="G40" s="1">
-        <v>3410422855355</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>230</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="2">
-        <v>9471</v>
-      </c>
-      <c r="D41" s="3">
-        <v>3310427995945</v>
+        <v>231</v>
+      </c>
+      <c r="C41">
+        <v>4734</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1550202253853</v>
       </c>
       <c r="E41" t="b">
         <v>1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" s="1">
-        <v>3310427775945</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>225</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="2">
-        <v>8534</v>
-      </c>
-      <c r="D42" s="3">
-        <v>3420286011893</v>
+        <v>226</v>
+      </c>
+      <c r="C42">
+        <v>5100</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1730177320361</v>
       </c>
       <c r="E42" t="b">
         <v>1</v>
-      </c>
-      <c r="F42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G42" s="1">
-        <v>3420286011843</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>225</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="2">
-        <v>88</v>
-      </c>
-      <c r="D43" s="3">
-        <v>3310007903593</v>
+        <v>227</v>
+      </c>
+      <c r="C43">
+        <v>5103</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1730115833823</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G43" s="1">
-        <v>3310070790359</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D44" s="3">
-        <v>3310022222945</v>
+        <v>229</v>
+      </c>
+      <c r="C44">
+        <v>5111</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1730131684495</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>60</v>
-      </c>
-      <c r="G44" s="1">
-        <v>3310024229145</v>
-      </c>
-      <c r="H44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="2">
-        <v>8970</v>
-      </c>
-      <c r="D45" s="3">
-        <v>3410161662055</v>
+        <v>137</v>
+      </c>
+      <c r="C45">
+        <v>5555</v>
+      </c>
+      <c r="D45" s="1">
+        <v>3310404721113</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>59</v>
-      </c>
-      <c r="G45" s="1">
-        <v>3410163662055</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D46" s="3">
-        <v>3520113155410</v>
+        <v>138</v>
+      </c>
+      <c r="C46">
+        <v>5556</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3310446365177</v>
       </c>
       <c r="E46" t="b">
         <v>1</v>
@@ -2302,16 +2482,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D47" s="3">
-        <v>3720113176898</v>
+        <v>198</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3310622873309</v>
       </c>
       <c r="E47" t="b">
         <v>1</v>
@@ -2319,39 +2499,42 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C48" s="2">
-        <v>9103</v>
-      </c>
-      <c r="D48" s="3">
-        <v>3430130408902</v>
+        <v>-9999</v>
+      </c>
+      <c r="D48" s="1">
+        <v>3310022222945</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G48" s="1">
-        <v>3430130408907</v>
+        <v>3310024229145</v>
+      </c>
+      <c r="H48" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C49" s="2">
-        <v>3032</v>
-      </c>
-      <c r="D49" s="3">
-        <v>3730333449105</v>
+        <v>-9999</v>
+      </c>
+      <c r="D49" s="1">
+        <v>3310094278359</v>
       </c>
       <c r="E49" t="b">
         <v>1</v>
@@ -2360,30 +2543,24 @@
         <v>59</v>
       </c>
       <c r="G49" s="1">
-        <v>3730333448105</v>
+        <v>3310094218359</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D50" s="3">
-        <v>3120103577449</v>
+        <v>185</v>
+      </c>
+      <c r="C50">
+        <v>-9999</v>
+      </c>
+      <c r="D50" s="1">
+        <v>3310006820009</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>60</v>
-      </c>
-      <c r="G50" s="1">
-        <v>3120103577449</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2396,7 +2573,7 @@
       <c r="C51" s="2">
         <v>5841</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="1">
         <v>3330320673357</v>
       </c>
       <c r="E51" t="b">
@@ -2414,62 +2591,56 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="3">
-        <v>3120197324509</v>
+        <v>144</v>
+      </c>
+      <c r="C52">
+        <v>5878</v>
+      </c>
+      <c r="D52" s="1">
+        <v>3330285935626</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>60</v>
-      </c>
-      <c r="G52" s="1">
-        <v>3120197324509</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C53" s="2">
-        <v>7853</v>
-      </c>
-      <c r="D53" s="3">
-        <v>3120244368991</v>
+        <v>-9999</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3520233441959</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G53" s="1">
-        <v>3120244368991</v>
+        <v>3520252451959</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D54" s="3">
-        <v>3630274228586</v>
+        <v>129</v>
+      </c>
+      <c r="C54">
+        <v>-9999</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3524012906315</v>
       </c>
       <c r="E54" t="b">
         <v>1</v>
@@ -2477,281 +2648,1530 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="3">
-        <v>3630297069351</v>
+        <v>133</v>
+      </c>
+      <c r="C55">
+        <v>6308</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3520113520899</v>
       </c>
       <c r="E55" t="b">
         <v>1</v>
-      </c>
-      <c r="F55" t="s">
-        <v>59</v>
-      </c>
-      <c r="G55" s="1">
-        <v>3630297009391</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D56" s="3">
-        <v>3630224801051</v>
+        <v>145</v>
+      </c>
+      <c r="C56">
+        <v>6321</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1482691735201</v>
       </c>
       <c r="E56" t="b">
         <v>1</v>
-      </c>
-      <c r="F56" t="s">
-        <v>59</v>
-      </c>
-      <c r="G56" s="1">
-        <v>3630224801851</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D57" s="3">
-        <v>3540169000129</v>
+        <v>147</v>
+      </c>
+      <c r="C57">
+        <v>6322</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3520229170131</v>
       </c>
       <c r="E57" t="b">
         <v>1</v>
-      </c>
-      <c r="F57" t="s">
-        <v>59</v>
-      </c>
-      <c r="G57" s="1">
-        <v>3540169800129</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
-      </c>
-      <c r="C58" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D58" s="3">
-        <v>6116186586471</v>
+        <v>186</v>
+      </c>
+      <c r="C58">
+        <v>-9999</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3520250795985</v>
       </c>
       <c r="E58" t="b">
         <v>1</v>
-      </c>
-      <c r="F58" t="s">
-        <v>59</v>
-      </c>
-      <c r="G58" s="1">
-        <v>6110186586471</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="2">
-        <v>8142</v>
-      </c>
-      <c r="D59" s="3">
-        <v>2330147913947</v>
+        <v>187</v>
+      </c>
+      <c r="C59">
+        <v>6332</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3520278197568</v>
       </c>
       <c r="E59" t="b">
         <v>1</v>
-      </c>
-      <c r="F59" t="s">
-        <v>59</v>
-      </c>
-      <c r="G59" s="1">
-        <v>3230147913947</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
-      </c>
-      <c r="C60" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D60" s="3">
-        <v>3230239609409</v>
+        <v>189</v>
+      </c>
+      <c r="C60">
+        <v>6347</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3520220079939</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>59</v>
-      </c>
-      <c r="G60" s="1">
-        <v>3230243960949</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
-      </c>
-      <c r="C61" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D61" s="3">
-        <v>3310094278359</v>
+        <v>179</v>
+      </c>
+      <c r="C61">
+        <v>-9999</v>
+      </c>
+      <c r="D61" s="1">
+        <v>3520278901079</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
-      </c>
-      <c r="F61" t="s">
-        <v>59</v>
-      </c>
-      <c r="G61" s="1">
-        <v>3310094218359</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
-      </c>
-      <c r="C62" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D62" s="3">
-        <v>3712124627410</v>
+        <v>159</v>
+      </c>
+      <c r="C62">
+        <v>-9999</v>
+      </c>
+      <c r="D62" s="1">
+        <v>3530307572877</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>59</v>
-      </c>
-      <c r="G62" s="1">
-        <v>3710212462741</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>208</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="2">
-        <v>8421</v>
-      </c>
-      <c r="D63" s="3">
-        <v>3520130596129</v>
+        <v>209</v>
+      </c>
+      <c r="C63">
+        <v>-9999</v>
+      </c>
+      <c r="D63" s="1">
+        <v>3530175006143</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
-      </c>
-      <c r="F63" t="s">
-        <v>59</v>
-      </c>
-      <c r="G63" s="1">
-        <v>3520130596139</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64">
+        <v>-9999</v>
+      </c>
+      <c r="D64" s="1">
+        <v>3530119734885</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>113</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>114</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C65" s="2">
         <v>7123</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D65" s="1">
         <v>3250084585115</v>
       </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>59</v>
-      </c>
-      <c r="G64" s="1">
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>59</v>
+      </c>
+      <c r="G65" s="1">
         <v>3520084585115</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>115</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>116</v>
       </c>
-      <c r="C65" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="D65" s="3">
+      <c r="C66" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D66" s="1">
         <v>3650260757017</v>
       </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>59</v>
-      </c>
-      <c r="G65" s="1">
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" s="1">
         <v>3650260787517</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>117</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>118</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C67" s="2">
         <v>7168</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D67" s="1">
         <v>3650243097025</v>
       </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
-        <v>59</v>
-      </c>
-      <c r="G66" s="1">
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>59</v>
+      </c>
+      <c r="G67" s="1">
         <v>3650243291025</v>
       </c>
     </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68">
+        <v>7215</v>
+      </c>
+      <c r="D68" s="1">
+        <v>3650109512843</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69">
+        <v>7240</v>
+      </c>
+      <c r="D69" s="1">
+        <v>3630296393117</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>232</v>
+      </c>
+      <c r="B70" t="s">
+        <v>233</v>
+      </c>
+      <c r="C70">
+        <v>-9999</v>
+      </c>
+      <c r="D70" s="1">
+        <v>3520013745507</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71">
+        <v>7489</v>
+      </c>
+      <c r="D71" s="1">
+        <v>3620105625631</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D72" s="1">
+        <v>3720212416532</v>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>59</v>
+      </c>
+      <c r="G72" s="1">
+        <v>3120212416532</v>
+      </c>
+      <c r="H72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3120203176499</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>60</v>
+      </c>
+      <c r="G73" s="3">
+        <v>3120203176499</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D74" s="1">
+        <v>3120202690303</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>60</v>
+      </c>
+      <c r="G74" s="3">
+        <v>3120202690303</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" t="s">
+        <v>66</v>
+      </c>
+      <c r="C75" s="2">
+        <v>7801</v>
+      </c>
+      <c r="D75" s="1">
+        <v>3120558226560</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>59</v>
+      </c>
+      <c r="G75" s="1">
+        <v>3120258226560</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D76" s="1">
+        <v>3120103577449</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>60</v>
+      </c>
+      <c r="G76" s="1">
+        <v>3120103577449</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D77" s="1">
+        <v>3120197324509</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>60</v>
+      </c>
+      <c r="G77" s="1">
+        <v>3120197324509</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>88</v>
+      </c>
+      <c r="B78" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" s="2">
+        <v>7853</v>
+      </c>
+      <c r="D78" s="1">
+        <v>3120244368991</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>60</v>
+      </c>
+      <c r="G78" s="1">
+        <v>3120244368991</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>172</v>
+      </c>
+      <c r="B79" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79">
+        <v>-9999</v>
+      </c>
+      <c r="D79" s="1">
+        <v>3730123850135</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>53</v>
+      </c>
+      <c r="B80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3520228850587</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
+        <v>59</v>
+      </c>
+      <c r="G80" s="3">
+        <v>3520228850581</v>
+      </c>
+      <c r="H80" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81">
+        <v>-9999</v>
+      </c>
+      <c r="D81" s="1">
+        <v>3730139208949</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="2">
+        <v>8099</v>
+      </c>
+      <c r="D82" s="1">
+        <v>3330416456315</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>59</v>
+      </c>
+      <c r="G82" s="1">
+        <v>3230416456315</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="2">
+        <v>8082</v>
+      </c>
+      <c r="D83" s="1">
+        <v>3230460778535</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>60</v>
+      </c>
+      <c r="G83" s="3">
+        <v>3230460778535</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="2">
+        <v>8096</v>
+      </c>
+      <c r="D84" s="1">
+        <v>3230425492523</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>59</v>
+      </c>
+      <c r="G84" s="1">
+        <v>3230425492253</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D85" s="1">
+        <v>3230968844001</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>59</v>
+      </c>
+      <c r="G85" s="1">
+        <v>3230468844001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="2">
+        <v>8001</v>
+      </c>
+      <c r="D86" s="1">
+        <v>3234564196655</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>59</v>
+      </c>
+      <c r="G86" s="1">
+        <v>3230456419665</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>25</v>
+      </c>
+      <c r="B87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D87" s="1">
+        <v>2330492812615</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
+        <v>59</v>
+      </c>
+      <c r="G87" s="1">
+        <v>3230482812615</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" t="s">
+        <v>102</v>
+      </c>
+      <c r="C88" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D88" s="1">
+        <v>6116186586471</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
+        <v>59</v>
+      </c>
+      <c r="G88" s="1">
+        <v>6110186586471</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" s="2">
+        <v>8142</v>
+      </c>
+      <c r="D89" s="1">
+        <v>2330147913947</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" t="s">
+        <v>59</v>
+      </c>
+      <c r="G89" s="1">
+        <v>3230147913947</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D90" s="1">
+        <v>3230239609409</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="s">
+        <v>59</v>
+      </c>
+      <c r="G90" s="1">
+        <v>3230243960949</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>148</v>
+      </c>
+      <c r="B91" t="s">
+        <v>149</v>
+      </c>
+      <c r="C91">
+        <v>8170</v>
+      </c>
+      <c r="D91" s="1">
+        <v>2330916291721</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92">
+        <v>8163</v>
+      </c>
+      <c r="D92" s="1">
+        <v>3330603076765</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>151</v>
+      </c>
+      <c r="B93" t="s">
+        <v>152</v>
+      </c>
+      <c r="C93">
+        <v>-9999</v>
+      </c>
+      <c r="D93" s="1">
+        <v>3230907418837</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>151</v>
+      </c>
+      <c r="B94" t="s">
+        <v>153</v>
+      </c>
+      <c r="C94">
+        <v>8202</v>
+      </c>
+      <c r="D94" s="1">
+        <v>3230343174775</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>151</v>
+      </c>
+      <c r="B95" t="s">
+        <v>154</v>
+      </c>
+      <c r="C95">
+        <v>-9999</v>
+      </c>
+      <c r="D95" s="1">
+        <v>3230364889181</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="2">
+        <v>8253</v>
+      </c>
+      <c r="D96" s="1">
+        <v>3220364078687</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>59</v>
+      </c>
+      <c r="G96" s="1">
+        <v>3220364078087</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>111</v>
+      </c>
+      <c r="B97" t="s">
+        <v>112</v>
+      </c>
+      <c r="C97" s="2">
+        <v>8421</v>
+      </c>
+      <c r="D97" s="1">
+        <v>3520130596129</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>59</v>
+      </c>
+      <c r="G97" s="1">
+        <v>3520130596139</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" s="2">
+        <v>8468</v>
+      </c>
+      <c r="D98" s="1">
+        <v>3240486787951</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
+        <v>59</v>
+      </c>
+      <c r="G98" s="1">
+        <v>3240480787951</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>109</v>
+      </c>
+      <c r="B99" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D99" s="1">
+        <v>3712124627410</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>59</v>
+      </c>
+      <c r="G99" s="1">
+        <v>3710212462741</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100">
+        <v>8486</v>
+      </c>
+      <c r="D100" s="1">
+        <v>3420104746687</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101" t="s">
+        <v>127</v>
+      </c>
+      <c r="C101">
+        <v>-9999</v>
+      </c>
+      <c r="D101" s="1">
+        <v>3420208441818</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>74</v>
+      </c>
+      <c r="B102" t="s">
+        <v>75</v>
+      </c>
+      <c r="C102" s="2">
+        <v>8534</v>
+      </c>
+      <c r="D102" s="1">
+        <v>3420286011893</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>59</v>
+      </c>
+      <c r="G102" s="1">
+        <v>3420286011843</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>55</v>
+      </c>
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D103" s="1">
+        <v>3520241959731</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>59</v>
+      </c>
+      <c r="G103" s="1">
+        <v>3420241959731</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" t="s">
+        <v>57</v>
+      </c>
+      <c r="C104" s="2">
+        <v>8547</v>
+      </c>
+      <c r="D104" s="1">
+        <v>3420206866313</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>59</v>
+      </c>
+      <c r="G104" s="1">
+        <v>3420206866713</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105" t="s">
+        <v>58</v>
+      </c>
+      <c r="C105" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D105" s="1">
+        <v>9110901034965</v>
+      </c>
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" t="s">
+        <v>59</v>
+      </c>
+      <c r="G105" s="1">
+        <v>9110901034695</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>70</v>
+      </c>
+      <c r="B106" t="s">
+        <v>71</v>
+      </c>
+      <c r="C106" s="2">
+        <v>8771</v>
+      </c>
+      <c r="D106" s="1">
+        <v>3410422858955</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>59</v>
+      </c>
+      <c r="G106" s="1">
+        <v>3410422855355</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" t="s">
+        <v>191</v>
+      </c>
+      <c r="C107">
+        <v>8870</v>
+      </c>
+      <c r="D107" s="1">
+        <v>3410205451655</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>80</v>
+      </c>
+      <c r="B108" t="s">
+        <v>81</v>
+      </c>
+      <c r="C108" s="2">
+        <v>8970</v>
+      </c>
+      <c r="D108" s="1">
+        <v>3410161662055</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" t="s">
+        <v>59</v>
+      </c>
+      <c r="G108" s="1">
+        <v>3410163662055</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" t="s">
+        <v>215</v>
+      </c>
+      <c r="C109">
+        <v>9027</v>
+      </c>
+      <c r="D109" s="1">
+        <v>3940201750849</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>216</v>
+      </c>
+      <c r="B110" t="s">
+        <v>217</v>
+      </c>
+      <c r="C110">
+        <v>9038</v>
+      </c>
+      <c r="D110" s="1">
+        <v>3520375772825</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" t="s">
+        <v>85</v>
+      </c>
+      <c r="C111" s="2">
+        <v>9103</v>
+      </c>
+      <c r="D111" s="1">
+        <v>3430130408902</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="s">
+        <v>59</v>
+      </c>
+      <c r="G111" s="1">
+        <v>3430130408907</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>180</v>
+      </c>
+      <c r="B112" t="s">
+        <v>181</v>
+      </c>
+      <c r="C112">
+        <v>-9999</v>
+      </c>
+      <c r="D112" s="1">
+        <v>3810160723793</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B113" t="s">
+        <v>16</v>
+      </c>
+      <c r="C113" s="2">
+        <v>9441</v>
+      </c>
+      <c r="D113" s="1">
+        <v>3310147826873</v>
+      </c>
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" t="s">
+        <v>59</v>
+      </c>
+      <c r="G113" s="1">
+        <v>3310147896873</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>72</v>
+      </c>
+      <c r="B114" t="s">
+        <v>73</v>
+      </c>
+      <c r="C114" s="2">
+        <v>9471</v>
+      </c>
+      <c r="D114" s="1">
+        <v>3310427995945</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" t="s">
+        <v>59</v>
+      </c>
+      <c r="G114" s="1">
+        <v>3310427775945</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>18</v>
+      </c>
+      <c r="C115" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D115" s="1">
+        <v>3460357085705</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>59</v>
+      </c>
+      <c r="G115" s="1">
+        <v>3460357086705</v>
+      </c>
+      <c r="H115" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" t="s">
+        <v>31</v>
+      </c>
+      <c r="C116" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D116" s="1">
+        <v>3310074119078</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>59</v>
+      </c>
+      <c r="G116" s="1">
+        <v>3310074119878</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>17</v>
+      </c>
+      <c r="B117" t="s">
+        <v>41</v>
+      </c>
+      <c r="C117" s="2">
+        <v>558</v>
+      </c>
+      <c r="D117" s="1">
+        <v>3530020775569</v>
+      </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" t="s">
+        <v>46</v>
+      </c>
+      <c r="C118" s="2">
+        <v>175</v>
+      </c>
+      <c r="D118" s="1">
+        <v>3330332918642</v>
+      </c>
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+      <c r="F118" t="s">
+        <v>59</v>
+      </c>
+      <c r="G118" s="1">
+        <v>3330382918642</v>
+      </c>
+      <c r="H118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>17</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D119" s="1">
+        <v>6110119162492</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>17</v>
+      </c>
+      <c r="B120" t="s">
+        <v>67</v>
+      </c>
+      <c r="C120" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D120" s="1">
+        <v>3460107505057</v>
+      </c>
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>17</v>
+      </c>
+      <c r="B121" t="s">
+        <v>82</v>
+      </c>
+      <c r="C121" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D121" s="1">
+        <v>3520113155410</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" t="s">
+        <v>83</v>
+      </c>
+      <c r="C122" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D122" s="1">
+        <v>3720113176898</v>
+      </c>
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>17</v>
+      </c>
+      <c r="B123" t="s">
+        <v>95</v>
+      </c>
+      <c r="C123" s="2">
+        <v>-9999</v>
+      </c>
+      <c r="D123" s="1">
+        <v>3630274228586</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" t="s">
+        <v>141</v>
+      </c>
+      <c r="C124">
+        <v>-9999</v>
+      </c>
+      <c r="D124" s="1">
+        <v>3040320000444</v>
+      </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" t="s">
+        <v>160</v>
+      </c>
+      <c r="C125">
+        <v>-9999</v>
+      </c>
+      <c r="D125" s="1">
+        <v>3740269243100</v>
+      </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" t="s">
+        <v>161</v>
+      </c>
+      <c r="C126">
+        <v>-9999</v>
+      </c>
+      <c r="D126" s="1">
+        <v>3710139208948</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>17</v>
+      </c>
+      <c r="B127" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127">
+        <v>-9999</v>
+      </c>
+      <c r="D127" s="1">
+        <v>3520216284084</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>17</v>
+      </c>
+      <c r="B128" t="s">
+        <v>182</v>
+      </c>
+      <c r="C128">
+        <v>-9999</v>
+      </c>
+      <c r="D128" s="1">
+        <v>3130389293402</v>
+      </c>
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" t="s">
+        <v>183</v>
+      </c>
+      <c r="C129">
+        <v>-9999</v>
+      </c>
+      <c r="D129" s="1">
+        <v>3520210275826</v>
+      </c>
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" t="s">
+        <v>196</v>
+      </c>
+      <c r="C130">
+        <v>-9999</v>
+      </c>
+      <c r="D130" s="1">
+        <v>3520112184680</v>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H130">
+    <sortState ref="A2:H130">
+      <sortCondition ref="A1:A130"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>